<commit_message>
Changes for version 25.1205.3923 (Export G-code)
First version of G-code export is tested and working.
</commit_message>
<xml_diff>
--- a/Docs/ShopToolsWorksheet.xlsx
+++ b/Docs/ShopToolsWorksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48df8f255f7bda56/Develop/Shared/ShopTools/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1970" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08350562-DBF5-4B61-8CD9-E7E059C47A1B}"/>
+  <xr:revisionPtr revIDLastSave="1973" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1E5A308-3463-499E-A80B-BB8462FB4610}"/>
   <bookViews>
-    <workbookView xWindow="5496" yWindow="2652" windowWidth="17256" windowHeight="8964" firstSheet="4" activeTab="4" xr2:uid="{66387098-6DAB-4DD6-BA63-A47627A5E346}"/>
+    <workbookView xWindow="5496" yWindow="2652" windowWidth="17256" windowHeight="8964" firstSheet="3" activeTab="3" xr2:uid="{66387098-6DAB-4DD6-BA63-A47627A5E346}"/>
   </bookViews>
   <sheets>
     <sheet name="frmMain" sheetId="9" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="WorkpieceInfoItem" sheetId="18" r:id="rId17"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">OperationActionTypes!$A$1:$I$33</definedName>
     <definedName name="polarizationLength">Polarization!$E$2</definedName>
     <definedName name="polarizationWidth">Polarization!$F$2</definedName>
     <definedName name="polarizationWkHeight">Polarization!$L$2</definedName>
@@ -5589,11 +5590,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D95A485-D9E0-44E7-A352-6F438C309CFE}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -5624,7 +5626,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -5652,7 +5654,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawCircleCenterDiameter&lt;/td&gt;&lt;td&gt;X, Y, Diameter&lt;/td&gt;&lt;td&gt;Draw a circle using a center reference point and diameter.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -5680,7 +5682,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawCircleCenterRadius&lt;/td&gt;&lt;td&gt;X, Y, Radius&lt;/td&gt;&lt;td&gt;Draw a circle using a center reference point and radius.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -5705,7 +5707,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawCircleDiameter&lt;/td&gt;&lt;td&gt;X, Y, Diameter&lt;/td&gt;&lt;td&gt;Draw a circle using corner X, Y references and diameter.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -5730,7 +5732,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawCircleRadius&lt;/td&gt;&lt;td&gt;X, Y, Radius&lt;/td&gt;&lt;td&gt;Draw a circle using corner X, Y references and radius.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -5761,7 +5763,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawEllipseCenterDiameterXY&lt;/td&gt;&lt;td&gt;X, Y, DiameterX, DiameterY&lt;/td&gt;&lt;td&gt;Draw an ellipse using a center reference point and independent diameters.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -5792,7 +5794,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawEllipseCenterRadiusXY&lt;/td&gt;&lt;td&gt;X, Y, RadiusX, RadiusY&lt;/td&gt;&lt;td&gt;Draw an ellipse using a center reference point and independent radii.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -5820,7 +5822,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawEllipseDiameterXY&lt;/td&gt;&lt;td&gt;X, Y, DiameterX, DiameterY&lt;/td&gt;&lt;td&gt;Draw an ellipse using corner X, Y references and independent diameters.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -5848,7 +5850,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawEllipseLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Draw an ellipse using corner X, Y starting references, length, and width.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -5876,7 +5878,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawEllipseRadiusXY&lt;/td&gt;&lt;td&gt;X, Y, RadiusX, RadiusY&lt;/td&gt;&lt;td&gt;Draw an ellipse using corner X, Y references and independent radii.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -5901,7 +5903,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawEllipseXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Draw an ellipse using starting and ending X, Y coordinates.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -5929,7 +5931,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawLineAngleLength&lt;/td&gt;&lt;td&gt;X, Y, Angle, Length&lt;/td&gt;&lt;td&gt;Draw a line using a point, an angle, and a length.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -5957,7 +5959,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawLineLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Draw a line using a point, a length, and a width.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -5982,7 +5984,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawLineXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Draw a line using two points.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -6004,7 +6006,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawPath&lt;/td&gt;&lt;td&gt;PathData&lt;/td&gt;&lt;td&gt;Draw the path specified in the PathData property.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -6032,7 +6034,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawRectangleLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Draw a rectangle using a corner, length, and width.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -6057,7 +6059,7 @@
         <v>&lt;tr&gt;&lt;td&gt;DrawRectangleXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Draw a rectangle using two corner points.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -6085,7 +6087,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillCircleCenterDiameter&lt;/td&gt;&lt;td&gt;X, Y, Diameter&lt;/td&gt;&lt;td&gt;Fill a circle using the center reference and a diameter.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -6113,7 +6115,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillCircleCenterRadius&lt;/td&gt;&lt;td&gt;X, Y, Radius&lt;/td&gt;&lt;td&gt;Fill a circle using its center reference and a radius.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -6138,7 +6140,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillCircleDiameter&lt;/td&gt;&lt;td&gt;X, Y, Diameter&lt;/td&gt;&lt;td&gt;Fill a circle using its corner reference and a diameter.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -6163,7 +6165,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillCircleRadius&lt;/td&gt;&lt;td&gt;X, Y, Radius&lt;/td&gt;&lt;td&gt;Fill a circle using its corner reference and a radius.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -6194,7 +6196,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillEllipseCenterDiameterXY&lt;/td&gt;&lt;td&gt;X, Y, DiameterX, DiameterY&lt;/td&gt;&lt;td&gt;Fill an ellipse using a center reference point and independent diameter values.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -6225,7 +6227,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillEllipseCenterRadiusXY&lt;/td&gt;&lt;td&gt;X, Y, RadiusX, RadiusY&lt;/td&gt;&lt;td&gt;Fill an ellipse using a center reference point and independent radii.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -6253,7 +6255,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillEllipseDiameterXY&lt;/td&gt;&lt;td&gt;X, Y, DiameterX, DiameterY&lt;/td&gt;&lt;td&gt;Fill an ellipse using a corner point and independent diameter values.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -6281,7 +6283,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillEllipseLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Fill an ellipse using corner X, Y starting references, length, and width.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -6309,7 +6311,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillEllipseRadiusXY&lt;/td&gt;&lt;td&gt;X, Y, RadiusX, RadiusY&lt;/td&gt;&lt;td&gt;Fill an ellipse using a corner point and independent radii.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -6334,7 +6336,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillEllipseXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Fill an ellipse using starting and ending X, Y coordinates.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -6356,7 +6358,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillPath&lt;/td&gt;&lt;td&gt;PathData&lt;/td&gt;&lt;td&gt;Fill the path specified in the PathData property.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -6384,7 +6386,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillRectangleLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Fill a rectangle using one corner, width, and height.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -6409,7 +6411,7 @@
         <v>&lt;tr&gt;&lt;td&gt;FillRectangleXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Fill a rectangle using two corners.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -6479,6 +6481,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I33" xr:uid="{4D95A485-D9E0-44E7-A352-6F438C309CFE}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="X, Y"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6488,9 +6497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C11D7ED-A239-4470-B308-11D637DC39C8}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F23"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updates for version 25.1206.4151
</commit_message>
<xml_diff>
--- a/Docs/ShopToolsWorksheet.xlsx
+++ b/Docs/ShopToolsWorksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48df8f255f7bda56/Develop/Shared/ShopTools/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1973" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1E5A308-3463-499E-A80B-BB8462FB4610}"/>
+  <xr:revisionPtr revIDLastSave="2053" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC589ECF-8062-4366-AD0A-DAD0BCBB78FE}"/>
   <bookViews>
-    <workbookView xWindow="5496" yWindow="2652" windowWidth="17256" windowHeight="8964" firstSheet="3" activeTab="3" xr2:uid="{66387098-6DAB-4DD6-BA63-A47627A5E346}"/>
+    <workbookView xWindow="5496" yWindow="2652" windowWidth="17256" windowHeight="8964" firstSheet="14" activeTab="17" xr2:uid="{66387098-6DAB-4DD6-BA63-A47627A5E346}"/>
   </bookViews>
   <sheets>
     <sheet name="frmMain" sheetId="9" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="UserToolItem" sheetId="10" r:id="rId15"/>
     <sheet name="Polarization" sheetId="15" r:id="rId16"/>
     <sheet name="WorkpieceInfoItem" sheetId="18" r:id="rId17"/>
+    <sheet name="Work" sheetId="20" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">OperationActionTypes!$A$1:$I$33</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="591">
   <si>
     <t>Name</t>
   </si>
@@ -1778,6 +1779,60 @@
   </si>
   <si>
     <t>The start location of the router for this cut.</t>
+  </si>
+  <si>
+    <t>Transit</t>
+  </si>
+  <si>
+    <t>Start X</t>
+  </si>
+  <si>
+    <t>Start Y</t>
+  </si>
+  <si>
+    <t>End X</t>
+  </si>
+  <si>
+    <t>End Y</t>
+  </si>
+  <si>
+    <t>Plot</t>
+  </si>
+  <si>
+    <t>Adj Start X</t>
+  </si>
+  <si>
+    <t>Adj Start Y</t>
+  </si>
+  <si>
+    <t>Adj End X</t>
+  </si>
+  <si>
+    <t>Adj End Y</t>
+  </si>
+  <si>
+    <t>Diff Start X</t>
+  </si>
+  <si>
+    <t>Diff Start Y</t>
+  </si>
+  <si>
+    <t>Diff End X</t>
+  </si>
+  <si>
+    <t>Diff End Y</t>
+  </si>
+  <si>
+    <t>Next X</t>
+  </si>
+  <si>
+    <t>Next Y</t>
+  </si>
+  <si>
+    <t>Next End X</t>
+  </si>
+  <si>
+    <t>Next End Y</t>
   </si>
 </sst>
 </file>
@@ -4727,6 +4782,222 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E40DB11-6C4A-49D6-826F-B66B6B7A1415}">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C1" t="s">
+        <v>575</v>
+      </c>
+      <c r="D1" t="s">
+        <v>576</v>
+      </c>
+      <c r="E1" t="s">
+        <v>577</v>
+      </c>
+      <c r="F1" t="s">
+        <v>579</v>
+      </c>
+      <c r="G1" t="s">
+        <v>580</v>
+      </c>
+      <c r="H1" t="s">
+        <v>581</v>
+      </c>
+      <c r="I1" t="s">
+        <v>582</v>
+      </c>
+      <c r="J1" t="s">
+        <v>583</v>
+      </c>
+      <c r="K1" t="s">
+        <v>584</v>
+      </c>
+      <c r="L1" t="s">
+        <v>585</v>
+      </c>
+      <c r="M1" t="s">
+        <v>586</v>
+      </c>
+      <c r="N1" t="s">
+        <v>587</v>
+      </c>
+      <c r="O1" t="s">
+        <v>588</v>
+      </c>
+      <c r="P1" t="s">
+        <v>589</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>573</v>
+      </c>
+      <c r="B2">
+        <v>1301.75</v>
+      </c>
+      <c r="C2">
+        <v>609.6</v>
+      </c>
+      <c r="D2">
+        <v>1301.75</v>
+      </c>
+      <c r="E2">
+        <v>158.48500000000001</v>
+      </c>
+      <c r="F2">
+        <v>1301.75</v>
+      </c>
+      <c r="G2">
+        <v>609.6</v>
+      </c>
+      <c r="H2">
+        <v>1301.75</v>
+      </c>
+      <c r="I2">
+        <v>160.07249999999999</v>
+      </c>
+      <c r="J2">
+        <f>F2-B2</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:M2" si="0">G2-C2</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>1.5874999999999773</v>
+      </c>
+      <c r="N2">
+        <v>1301.75</v>
+      </c>
+      <c r="O2">
+        <v>160.07249999999999</v>
+      </c>
+      <c r="P2">
+        <v>1428.4849999999999</v>
+      </c>
+      <c r="Q2">
+        <v>160.07249999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>578</v>
+      </c>
+      <c r="B3">
+        <v>1301.75</v>
+      </c>
+      <c r="C3">
+        <v>158.48500000000001</v>
+      </c>
+      <c r="D3">
+        <v>1428.4849999999999</v>
+      </c>
+      <c r="E3">
+        <v>158.48500000000001</v>
+      </c>
+      <c r="F3">
+        <v>1301.75</v>
+      </c>
+      <c r="G3">
+        <v>160.07249999999999</v>
+      </c>
+      <c r="H3">
+        <v>1426.8974599999999</v>
+      </c>
+      <c r="I3">
+        <v>160.07249999999999</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J4" si="1">F3-B3</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K4" si="2">G3-C3</f>
+        <v>1.5874999999999773</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L4" si="3">H3-D3</f>
+        <v>-1.58753999999999</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M4" si="4">I3-E3</f>
+        <v>1.5874999999999773</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>578</v>
+      </c>
+      <c r="B4">
+        <v>1428.4849999999999</v>
+      </c>
+      <c r="C4">
+        <v>158.48500000000001</v>
+      </c>
+      <c r="D4">
+        <v>1428.4849999999999</v>
+      </c>
+      <c r="E4">
+        <v>609.6</v>
+      </c>
+      <c r="F4">
+        <v>1426.8974599999999</v>
+      </c>
+      <c r="G4">
+        <v>160.07249999999999</v>
+      </c>
+      <c r="H4">
+        <v>1426.8974599999999</v>
+      </c>
+      <c r="I4">
+        <v>609.6</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>-1.58753999999999</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>1.5874999999999773</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>-1.58753999999999</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2604EA-6AB7-4664-B3CE-D93FD89202ED}">
   <dimension ref="A1:G42"/>
@@ -5593,7 +5864,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
     </sheetView>

</xml_diff>

<commit_message>
Updates for version 25.1219.4900
Drawing support for all remaining shapes.
</commit_message>
<xml_diff>
--- a/Docs/ShopToolsWorksheet.xlsx
+++ b/Docs/ShopToolsWorksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48df8f255f7bda56/Develop/Shared/ShopTools/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2053" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC589ECF-8062-4366-AD0A-DAD0BCBB78FE}"/>
+  <xr:revisionPtr revIDLastSave="2327" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3AF5DD2-C24A-403D-9B37-CBDB4FC0EB36}"/>
   <bookViews>
-    <workbookView xWindow="5496" yWindow="2652" windowWidth="17256" windowHeight="8964" firstSheet="14" activeTab="17" xr2:uid="{66387098-6DAB-4DD6-BA63-A47627A5E346}"/>
+    <workbookView xWindow="4452" yWindow="1908" windowWidth="17256" windowHeight="8964" firstSheet="14" activeTab="17" xr2:uid="{66387098-6DAB-4DD6-BA63-A47627A5E346}"/>
   </bookViews>
   <sheets>
     <sheet name="frmMain" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="Work" sheetId="20" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">OperationActionTypes!$A$1:$I$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">OperationActionTypes!$A$1:$K$38</definedName>
     <definedName name="polarizationLength">Polarization!$E$2</definedName>
     <definedName name="polarizationWidth">Polarization!$F$2</definedName>
     <definedName name="polarizationWkHeight">Polarization!$L$2</definedName>
@@ -59,8 +59,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={D9896D3F-0395-4954-9833-6D67E23A01E0}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D9896D3F-0395-4954-9833-6D67E23A01E0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    For the OperationActionProperties list, see the PatternTemplatePlotProperties sheet.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="623">
   <si>
     <t>Name</t>
   </si>
@@ -1833,6 +1851,102 @@
   </si>
   <si>
     <t>Next End Y</t>
+  </si>
+  <si>
+    <t>The diameter of the shape.</t>
+  </si>
+  <si>
+    <t>The radius of the shape.</t>
+  </si>
+  <si>
+    <t>The X diameter of the shape.</t>
+  </si>
+  <si>
+    <t>The Y diameter of the shape.</t>
+  </si>
+  <si>
+    <t>The X radius of the shape.</t>
+  </si>
+  <si>
+    <t>The Y radius of the shape.</t>
+  </si>
+  <si>
+    <t>Arc</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>X, Y, Radius, StartAngle, EndAngle</t>
+  </si>
+  <si>
+    <t>Draw an arc using a center coordinate, an offset starting coordinate, and a sweep angle.</t>
+  </si>
+  <si>
+    <t>Draw an arc using a center coordinate, a radius, a start angle, and an end angle.</t>
+  </si>
+  <si>
+    <t>X, Y, X1, Y1, Angle</t>
+  </si>
+  <si>
+    <t>X, Y, X1, Y1, X2, Y2</t>
+  </si>
+  <si>
+    <t>Draw an arc from the specified start coordinate to the point nearest the specified end point, given the radius from the center to the starting offset.</t>
+  </si>
+  <si>
+    <t>StartAngle</t>
+  </si>
+  <si>
+    <t>EndAngle</t>
+  </si>
+  <si>
+    <t>The starting angle of the operation.</t>
+  </si>
+  <si>
+    <t>The ending angle of the operation.</t>
+  </si>
+  <si>
+    <t>The angle at which the operation begins.</t>
+  </si>
+  <si>
+    <t>The angle at which the operation ends.</t>
+  </si>
+  <si>
+    <t>Draw a rectangle using a center offset, length, and width.</t>
+  </si>
+  <si>
+    <t>Fill a rectangle using a center offset, length, and width.</t>
+  </si>
+  <si>
+    <t>Point A</t>
+  </si>
+  <si>
+    <t>Point B</t>
+  </si>
+  <si>
+    <t>Point C</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>ABAB</t>
+  </si>
+  <si>
+    <t>ACAB</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>result</t>
   </si>
 </sst>
 </file>
@@ -1868,7 +1982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1876,6 +1990,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1891,6 +2006,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Daniel Patterson" id="{DC0FD888-BADF-401B-BF0F-AF7FE88E8E42}" userId="48df8f255f7bda56" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2208,6 +2329,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2025-02-14T16:15:01.59" personId="{DC0FD888-BADF-401B-BF0F-AF7FE88E8E42}" id="{D9896D3F-0395-4954-9833-6D67E23A01E0}">
+    <text>For the OperationActionProperties list, see the PatternTemplatePlotProperties sheet.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A4320E-B37A-4B0E-8ACB-045DC2EF14B2}">
   <dimension ref="A1:G62"/>
@@ -4784,11 +4913,11 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E40DB11-6C4A-49D6-826F-B66B6B7A1415}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -4991,6 +5120,135 @@
       <c r="M4">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>614</v>
+      </c>
+      <c r="B7">
+        <v>1454</v>
+      </c>
+      <c r="C7">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>615</v>
+      </c>
+      <c r="B8">
+        <v>1454</v>
+      </c>
+      <c r="C8">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>616</v>
+      </c>
+      <c r="B9">
+        <v>1302</v>
+      </c>
+      <c r="C9">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>617</v>
+      </c>
+      <c r="B11">
+        <f>B8-B7</f>
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>C8-C7</f>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>618</v>
+      </c>
+      <c r="B12">
+        <f>B9-B7</f>
+        <v>-152</v>
+      </c>
+      <c r="C12">
+        <f>C9-C7</f>
+        <v>407</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>619</v>
+      </c>
+      <c r="B14">
+        <f>B11*B11+C11*C11</f>
+        <v>64516</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>620</v>
+      </c>
+      <c r="B15">
+        <f>B12*B11+C12*C11</f>
+        <v>103378</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>621</v>
+      </c>
+      <c r="B17">
+        <f>B15/B14</f>
+        <v>1.6023622047244095</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>622</v>
+      </c>
+      <c r="B19">
+        <f>B7+B11*B17</f>
+        <v>1454</v>
+      </c>
+      <c r="C19">
+        <f>C7+C11*B17</f>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1454.23</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1.6</v>
+      </c>
+      <c r="E22">
+        <f>A22+B22*C22</f>
+        <v>1454.23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>203</v>
+      </c>
+      <c r="B23">
+        <v>254</v>
+      </c>
+      <c r="C23">
+        <v>1.6</v>
+      </c>
+      <c r="E23">
+        <f>A23+B23*C23</f>
+        <v>609.40000000000009</v>
       </c>
     </row>
   </sheetData>
@@ -5861,12 +6119,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D95A485-D9E0-44E7-A352-6F438C309CFE}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -5874,111 +6131,134 @@
     <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.21875" customWidth="1"/>
+    <col min="8" max="8" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="60.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>597</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="str">
-        <f>CONCATENATE(A2,B2,C2,D2,E2)</f>
-        <v>DrawCircleCenterDiameter</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" t="str">
-        <f>CONCATENATE("&lt;tr&gt;&lt;td&gt;",F2,"&lt;/td&gt;&lt;td&gt;",G2,"&lt;/td&gt;&lt;td&gt;",H2,"&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;DrawCircleCenterDiameter&lt;/td&gt;&lt;td&gt;X, Y, Diameter&lt;/td&gt;&lt;td&gt;Draw a circle using a center reference point and diameter.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>454</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="str">
+        <f>CONCATENATE(A2,B2,C2,D2,E2,F2,G2)</f>
+        <v>DrawArcCenterOffsetXY</v>
+      </c>
+      <c r="I2" t="s">
+        <v>604</v>
+      </c>
+      <c r="J2" t="s">
+        <v>605</v>
+      </c>
+      <c r="K2" t="str">
+        <f>CONCATENATE("&lt;tr&gt;&lt;td&gt;",H2,"&lt;/td&gt;&lt;td&gt;",I2,"&lt;/td&gt;&lt;td&gt;",J2,"&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;DrawArcCenterOffsetXY&lt;/td&gt;&lt;td&gt;X, Y, X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Draw an arc from the specified start coordinate to the point nearest the specified end point, given the radius from the center to the starting offset.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>597</v>
       </c>
       <c r="C3" t="s">
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F33" si="0">CONCATENATE(A3,B3,C3,D3,E3)</f>
-        <v>DrawCircleCenterRadius</v>
-      </c>
-      <c r="G3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I33" si="1">CONCATENATE("&lt;tr&gt;&lt;td&gt;",F3,"&lt;/td&gt;&lt;td&gt;",G3,"&lt;/td&gt;&lt;td&gt;",H3,"&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;DrawCircleCenterRadius&lt;/td&gt;&lt;td&gt;X, Y, Radius&lt;/td&gt;&lt;td&gt;Draw a circle using a center reference point and radius.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>454</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="str">
+        <f>CONCATENATE(A3,B3,C3,D3,E3,F3,G3)</f>
+        <v>DrawArcCenterOffsetXYAngle</v>
+      </c>
+      <c r="I3" t="s">
+        <v>603</v>
+      </c>
+      <c r="J3" t="s">
+        <v>601</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K4" si="0">CONCATENATE("&lt;tr&gt;&lt;td&gt;",H3,"&lt;/td&gt;&lt;td&gt;",I3,"&lt;/td&gt;&lt;td&gt;",J3,"&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;DrawArcCenterOffsetXYAngle&lt;/td&gt;&lt;td&gt;X, Y, X1, Y1, Angle&lt;/td&gt;&lt;td&gt;Draw an arc using a center coordinate, an offset starting coordinate, and a sweep angle.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>597</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="str">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>598</v>
+      </c>
+      <c r="F4" t="s">
+        <v>599</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="str">
+        <f>CONCATENATE(A4,B4,C4,D4,E4,F4,G4)</f>
+        <v>DrawArcCenterRadiusStartEndAngle</v>
+      </c>
+      <c r="I4" t="s">
+        <v>600</v>
+      </c>
+      <c r="J4" t="s">
+        <v>602</v>
+      </c>
+      <c r="K4" t="str">
         <f t="shared" si="0"/>
-        <v>DrawCircleDiameter</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawCircleDiameter&lt;/td&gt;&lt;td&gt;X, Y, Diameter&lt;/td&gt;&lt;td&gt;Draw a circle using corner X, Y references and diameter.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>&lt;tr&gt;&lt;td&gt;DrawArcCenterRadiusStartEndAngle&lt;/td&gt;&lt;td&gt;X, Y, Radius, StartAngle, EndAngle&lt;/td&gt;&lt;td&gt;Draw an arc using a center coordinate, a radius, a start angle, and an end angle.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -5986,114 +6266,105 @@
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>DrawCircleRadius</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawCircleRadius&lt;/td&gt;&lt;td&gt;X, Y, Radius&lt;/td&gt;&lt;td&gt;Draw a circle using corner X, Y references and radius.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" ref="H5:H38" si="1">CONCATENATE(A5,B5,C5,D5,E5,F5,G5)</f>
+        <v>DrawCircleCenterDiameter</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" t="str">
+        <f>CONCATENATE("&lt;tr&gt;&lt;td&gt;",H5,"&lt;/td&gt;&lt;td&gt;",I5,"&lt;/td&gt;&lt;td&gt;",J5,"&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;DrawCircleCenterDiameter&lt;/td&gt;&lt;td&gt;X, Y, Diameter&lt;/td&gt;&lt;td&gt;Draw a circle using a center reference point and diameter.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>DrawEllipseCenterDiameterXY</v>
-      </c>
-      <c r="G6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" t="str">
+        <v>23</v>
+      </c>
+      <c r="H6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawEllipseCenterDiameterXY&lt;/td&gt;&lt;td&gt;X, Y, DiameterX, DiameterY&lt;/td&gt;&lt;td&gt;Draw an ellipse using a center reference point and independent diameters.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>DrawCircleCenterRadius</v>
+      </c>
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" ref="K6:K38" si="2">CONCATENATE("&lt;tr&gt;&lt;td&gt;",H6,"&lt;/td&gt;&lt;td&gt;",I6,"&lt;/td&gt;&lt;td&gt;",J6,"&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;DrawCircleCenterRadius&lt;/td&gt;&lt;td&gt;X, Y, Radius&lt;/td&gt;&lt;td&gt;Draw a circle using a center reference point and radius.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>DrawEllipseCenterRadiusXY</v>
-      </c>
-      <c r="G7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" t="str">
+        <v>16</v>
+      </c>
+      <c r="H7" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawEllipseCenterRadiusXY&lt;/td&gt;&lt;td&gt;X, Y, RadiusX, RadiusY&lt;/td&gt;&lt;td&gt;Draw an ellipse using a center reference point and independent radii.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>DrawCircleDiameter</v>
+      </c>
+      <c r="I7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawCircleDiameter&lt;/td&gt;&lt;td&gt;X, Y, Diameter&lt;/td&gt;&lt;td&gt;Draw a circle using corner X, Y references and diameter.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>DrawEllipseDiameterXY</v>
-      </c>
-      <c r="G8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" t="str">
+        <v>23</v>
+      </c>
+      <c r="H8" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawEllipseDiameterXY&lt;/td&gt;&lt;td&gt;X, Y, DiameterX, DiameterY&lt;/td&gt;&lt;td&gt;Draw an ellipse using corner X, Y references and independent diameters.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>DrawCircleRadius</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawCircleRadius&lt;/td&gt;&lt;td&gt;X, Y, Radius&lt;/td&gt;&lt;td&gt;Draw a circle using corner X, Y references and radius.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -6101,27 +6372,30 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>DrawEllipseLengthWidth</v>
-      </c>
-      <c r="G9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" t="s">
-        <v>430</v>
-      </c>
-      <c r="I9" t="str">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawEllipseLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Draw an ellipse using corner X, Y starting references, length, and width.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>DrawEllipseCenterDiameterXY</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawEllipseCenterDiameterXY&lt;/td&gt;&lt;td&gt;X, Y, DiameterX, DiameterY&lt;/td&gt;&lt;td&gt;Draw an ellipse using a center reference point and independent diameters.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -6129,27 +6403,30 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>DrawEllipseRadiusXY</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>DrawEllipseCenterRadiusXY</v>
+      </c>
+      <c r="I10" t="s">
         <v>46</v>
       </c>
-      <c r="H10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawEllipseRadiusXY&lt;/td&gt;&lt;td&gt;X, Y, RadiusX, RadiusY&lt;/td&gt;&lt;td&gt;Draw an ellipse using corner X, Y references and independent radii.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawEllipseCenterRadiusXY&lt;/td&gt;&lt;td&gt;X, Y, RadiusX, RadiusY&lt;/td&gt;&lt;td&gt;Draw an ellipse using a center reference point and independent radii.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -6157,132 +6434,141 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>DrawEllipseXY</v>
-      </c>
-      <c r="G11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" t="s">
-        <v>431</v>
-      </c>
-      <c r="I11" t="str">
+      <c r="H11" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawEllipseXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Draw an ellipse using starting and ending X, Y coordinates.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>DrawEllipseDiameterXY</v>
+      </c>
+      <c r="I11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawEllipseDiameterXY&lt;/td&gt;&lt;td&gt;X, Y, DiameterX, DiameterY&lt;/td&gt;&lt;td&gt;Draw an ellipse using corner X, Y references and independent diameters.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>DrawLineAngleLength</v>
-      </c>
-      <c r="G12" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" t="s">
-        <v>59</v>
-      </c>
-      <c r="I12" t="str">
+        <v>36</v>
+      </c>
+      <c r="H12" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawLineAngleLength&lt;/td&gt;&lt;td&gt;X, Y, Angle, Length&lt;/td&gt;&lt;td&gt;Draw a line using a point, an angle, and a length.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>DrawEllipseLengthWidth</v>
+      </c>
+      <c r="I12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" t="s">
+        <v>430</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawEllipseLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Draw an ellipse using corner X, Y starting references, length, and width.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>DrawLineLengthWidth</v>
-      </c>
-      <c r="G13" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" t="s">
-        <v>60</v>
-      </c>
-      <c r="I13" t="str">
+        <v>32</v>
+      </c>
+      <c r="H13" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawLineLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Draw a line using a point, a length, and a width.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>DrawEllipseRadiusXY</v>
+      </c>
+      <c r="I13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawEllipseRadiusXY&lt;/td&gt;&lt;td&gt;X, Y, RadiusX, RadiusY&lt;/td&gt;&lt;td&gt;Draw an ellipse using corner X, Y references and independent radii.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
       </c>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>DrawLineXY</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>DrawEllipseXY</v>
+      </c>
+      <c r="I14" t="s">
         <v>49</v>
       </c>
-      <c r="H14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawLineXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Draw a line using two points.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>431</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawEllipseXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Draw an ellipse using starting and ending X, Y coordinates.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>DrawPath</v>
-      </c>
-      <c r="G15" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" t="str">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawPath&lt;/td&gt;&lt;td&gt;PathData&lt;/td&gt;&lt;td&gt;Draw the path specified in the PathData property.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>DrawLineAngleLength</v>
+      </c>
+      <c r="I15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawLineAngleLength&lt;/td&gt;&lt;td&gt;X, Y, Angle, Length&lt;/td&gt;&lt;td&gt;Draw a line using a point, an angle, and a length.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
         <v>33</v>
@@ -6290,158 +6576,160 @@
       <c r="D16" t="s">
         <v>36</v>
       </c>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>DrawRectangleLengthWidth</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>DrawLineLengthWidth</v>
+      </c>
+      <c r="I16" t="s">
         <v>48</v>
       </c>
-      <c r="H16" t="s">
-        <v>63</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawRectangleLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Draw a rectangle using a corner, length, and width.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawLineLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Draw a line using a point, a length, and a width.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>32</v>
       </c>
-      <c r="F17" t="str">
-        <f t="shared" si="0"/>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>DrawLineXY</v>
+      </c>
+      <c r="I17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawLineXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Draw a line using two points.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>DrawPath</v>
+      </c>
+      <c r="I18" t="s">
+        <v>73</v>
+      </c>
+      <c r="J18" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawPath&lt;/td&gt;&lt;td&gt;PathData&lt;/td&gt;&lt;td&gt;Draw the path specified in the PathData property.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>DrawRectangleCenterLengthWidth</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" t="s">
+        <v>612</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawRectangleCenterLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Draw a rectangle using a center offset, length, and width.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>DrawRectangleLengthWidth</v>
+      </c>
+      <c r="I20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;DrawRectangleLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Draw a rectangle using a corner, length, and width.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
         <v>DrawRectangleXY</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I21" t="s">
         <v>49</v>
       </c>
-      <c r="H17" t="s">
+      <c r="J21" t="s">
         <v>64</v>
       </c>
-      <c r="I17" t="str">
-        <f t="shared" si="1"/>
+      <c r="K21" t="str">
+        <f t="shared" si="2"/>
         <v>&lt;tr&gt;&lt;td&gt;DrawRectangleXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Draw a rectangle using two corner points.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>FillCircleCenterDiameter</v>
-      </c>
-      <c r="G18" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" t="s">
-        <v>65</v>
-      </c>
-      <c r="I18" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;FillCircleCenterDiameter&lt;/td&gt;&lt;td&gt;X, Y, Diameter&lt;/td&gt;&lt;td&gt;Fill a circle using the center reference and a diameter.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>FillCircleCenterRadius</v>
-      </c>
-      <c r="G19" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;FillCircleCenterRadius&lt;/td&gt;&lt;td&gt;X, Y, Radius&lt;/td&gt;&lt;td&gt;Fill a circle using its center reference and a radius.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v>FillCircleDiameter</v>
-      </c>
-      <c r="G20" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;FillCircleDiameter&lt;/td&gt;&lt;td&gt;X, Y, Diameter&lt;/td&gt;&lt;td&gt;Fill a circle using its corner reference and a diameter.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v>FillCircleRadius</v>
-      </c>
-      <c r="G21" t="s">
-        <v>44</v>
-      </c>
-      <c r="H21" t="s">
-        <v>68</v>
-      </c>
-      <c r="I21" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;FillCircleRadius&lt;/td&gt;&lt;td&gt;X, Y, Radius&lt;/td&gt;&lt;td&gt;Fill a circle using its corner reference and a radius.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
@@ -6449,30 +6737,27 @@
       <c r="D22" t="s">
         <v>16</v>
       </c>
-      <c r="E22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v>FillEllipseCenterDiameterXY</v>
-      </c>
-      <c r="G22" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" t="s">
-        <v>69</v>
-      </c>
-      <c r="I22" t="str">
+      <c r="H22" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;FillEllipseCenterDiameterXY&lt;/td&gt;&lt;td&gt;X, Y, DiameterX, DiameterY&lt;/td&gt;&lt;td&gt;Fill an ellipse using a center reference point and independent diameter values.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>FillCircleCenterDiameter</v>
+      </c>
+      <c r="I22" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" t="s">
+        <v>65</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;FillCircleCenterDiameter&lt;/td&gt;&lt;td&gt;X, Y, Diameter&lt;/td&gt;&lt;td&gt;Fill a circle using the center reference and a diameter.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
         <v>31</v>
@@ -6480,81 +6765,72 @@
       <c r="D23" t="s">
         <v>23</v>
       </c>
-      <c r="E23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v>FillEllipseCenterRadiusXY</v>
-      </c>
-      <c r="G23" t="s">
-        <v>46</v>
-      </c>
-      <c r="H23" t="s">
-        <v>70</v>
-      </c>
-      <c r="I23" t="str">
+      <c r="H23" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;FillEllipseCenterRadiusXY&lt;/td&gt;&lt;td&gt;X, Y, RadiusX, RadiusY&lt;/td&gt;&lt;td&gt;Fill an ellipse using a center reference point and independent radii.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>FillCircleCenterRadius</v>
+      </c>
+      <c r="I23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" t="s">
+        <v>66</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;FillCircleCenterRadius&lt;/td&gt;&lt;td&gt;X, Y, Radius&lt;/td&gt;&lt;td&gt;Fill a circle using its center reference and a radius.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
       </c>
-      <c r="D24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v>FillEllipseDiameterXY</v>
-      </c>
-      <c r="G24" t="s">
-        <v>45</v>
-      </c>
-      <c r="H24" t="s">
-        <v>71</v>
-      </c>
-      <c r="I24" t="str">
+      <c r="H24" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;FillEllipseDiameterXY&lt;/td&gt;&lt;td&gt;X, Y, DiameterX, DiameterY&lt;/td&gt;&lt;td&gt;Fill an ellipse using a corner point and independent diameter values.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>FillCircleDiameter</v>
+      </c>
+      <c r="I24" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" t="s">
+        <v>67</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;FillCircleDiameter&lt;/td&gt;&lt;td&gt;X, Y, Diameter&lt;/td&gt;&lt;td&gt;Fill a circle using its corner reference and a diameter.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" t="str">
-        <f t="shared" ref="F25" si="2">CONCATENATE(A25,B25,C25,D25,E25)</f>
-        <v>FillEllipseLengthWidth</v>
-      </c>
-      <c r="G25" t="s">
-        <v>48</v>
-      </c>
-      <c r="H25" t="s">
-        <v>432</v>
-      </c>
-      <c r="I25" t="str">
-        <f t="shared" ref="I25" si="3">CONCATENATE("&lt;tr&gt;&lt;td&gt;",F25,"&lt;/td&gt;&lt;td&gt;",G25,"&lt;/td&gt;&lt;td&gt;",H25,"&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;FillEllipseLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Fill an ellipse using corner X, Y starting references, length, and width.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v>FillCircleRadius</v>
+      </c>
+      <c r="I25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;FillCircleRadius&lt;/td&gt;&lt;td&gt;X, Y, Radius&lt;/td&gt;&lt;td&gt;Fill a circle using its corner reference and a radius.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -6562,27 +6838,30 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
         <v>32</v>
       </c>
-      <c r="F26" t="str">
-        <f t="shared" si="0"/>
-        <v>FillEllipseRadiusXY</v>
-      </c>
-      <c r="G26" t="s">
-        <v>46</v>
-      </c>
-      <c r="H26" t="s">
-        <v>72</v>
-      </c>
-      <c r="I26" t="str">
+      <c r="H26" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;FillEllipseRadiusXY&lt;/td&gt;&lt;td&gt;X, Y, RadiusX, RadiusY&lt;/td&gt;&lt;td&gt;Fill an ellipse using a corner point and independent radii.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>FillEllipseCenterDiameterXY</v>
+      </c>
+      <c r="I26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" t="s">
+        <v>69</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;FillEllipseCenterDiameterXY&lt;/td&gt;&lt;td&gt;X, Y, DiameterX, DiameterY&lt;/td&gt;&lt;td&gt;Fill an ellipse using a center reference point and independent diameter values.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -6590,51 +6869,63 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" t="s">
         <v>32</v>
       </c>
-      <c r="F27" t="str">
-        <f t="shared" ref="F27" si="4">CONCATENATE(A27,B27,C27,D27,E27)</f>
-        <v>FillEllipseXY</v>
-      </c>
-      <c r="G27" t="s">
-        <v>49</v>
-      </c>
-      <c r="H27" t="s">
-        <v>433</v>
-      </c>
-      <c r="I27" t="str">
-        <f t="shared" ref="I27" si="5">CONCATENATE("&lt;tr&gt;&lt;td&gt;",F27,"&lt;/td&gt;&lt;td&gt;",G27,"&lt;/td&gt;&lt;td&gt;",H27,"&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;FillEllipseXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Fill an ellipse using starting and ending X, Y coordinates.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v>FillEllipseCenterRadiusXY</v>
+      </c>
+      <c r="I27" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" t="s">
+        <v>70</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;FillEllipseCenterRadiusXY&lt;/td&gt;&lt;td&gt;X, Y, RadiusX, RadiusY&lt;/td&gt;&lt;td&gt;Fill an ellipse using a center reference point and independent radii.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" t="str">
-        <f t="shared" si="0"/>
-        <v>FillPath</v>
-      </c>
-      <c r="G28" t="s">
-        <v>73</v>
-      </c>
-      <c r="H28" t="s">
-        <v>74</v>
-      </c>
-      <c r="I28" t="str">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;FillPath&lt;/td&gt;&lt;td&gt;PathData&lt;/td&gt;&lt;td&gt;Fill the path specified in the PathData property.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>FillEllipseDiameterXY</v>
+      </c>
+      <c r="I28" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28" t="s">
+        <v>71</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;FillEllipseDiameterXY&lt;/td&gt;&lt;td&gt;X, Y, DiameterX, DiameterY&lt;/td&gt;&lt;td&gt;Fill an ellipse using a corner point and independent diameter values.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
         <v>33</v>
@@ -6642,135 +6933,261 @@
       <c r="D29" t="s">
         <v>36</v>
       </c>
-      <c r="F29" t="str">
-        <f t="shared" si="0"/>
-        <v>FillRectangleLengthWidth</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="H29" t="str">
+        <f t="shared" si="1"/>
+        <v>FillEllipseLengthWidth</v>
+      </c>
+      <c r="I29" t="s">
         <v>48</v>
       </c>
-      <c r="H29" t="s">
-        <v>75</v>
-      </c>
-      <c r="I29" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;FillRectangleLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Fill a rectangle using one corner, width, and height.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="J29" t="s">
+        <v>432</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" ref="K29" si="3">CONCATENATE("&lt;tr&gt;&lt;td&gt;",H29,"&lt;/td&gt;&lt;td&gt;",I29,"&lt;/td&gt;&lt;td&gt;",J29,"&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;FillEllipseLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Fill an ellipse using corner X, Y starting references, length, and width.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>39</v>
       </c>
       <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v>FillEllipseRadiusXY</v>
+      </c>
+      <c r="I30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J30" t="s">
+        <v>72</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;FillEllipseRadiusXY&lt;/td&gt;&lt;td&gt;X, Y, RadiusX, RadiusY&lt;/td&gt;&lt;td&gt;Fill an ellipse using a corner point and independent radii.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="1"/>
+        <v>FillEllipseXY</v>
+      </c>
+      <c r="I31" t="s">
+        <v>49</v>
+      </c>
+      <c r="J31" t="s">
+        <v>433</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" ref="K31" si="4">CONCATENATE("&lt;tr&gt;&lt;td&gt;",H31,"&lt;/td&gt;&lt;td&gt;",I31,"&lt;/td&gt;&lt;td&gt;",J31,"&lt;/td&gt;&lt;/tr&gt;")</f>
+        <v>&lt;tr&gt;&lt;td&gt;FillEllipseXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Fill an ellipse using starting and ending X, Y coordinates.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="1"/>
+        <v>FillPath</v>
+      </c>
+      <c r="I32" t="s">
+        <v>73</v>
+      </c>
+      <c r="J32" t="s">
+        <v>74</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;FillPath&lt;/td&gt;&lt;td&gt;PathData&lt;/td&gt;&lt;td&gt;Fill the path specified in the PathData property.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>FillRectangleCenterLengthWidth</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J33" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="1"/>
+        <v>FillRectangleLengthWidth</v>
+      </c>
+      <c r="I34" t="s">
+        <v>48</v>
+      </c>
+      <c r="J34" t="s">
+        <v>75</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;FillRectangleLengthWidth&lt;/td&gt;&lt;td&gt;X, Y, Length, Width&lt;/td&gt;&lt;td&gt;Fill a rectangle using one corner, width, and height.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
         <v>32</v>
       </c>
-      <c r="F30" t="str">
-        <f t="shared" si="0"/>
+      <c r="H35" t="str">
+        <f t="shared" si="1"/>
         <v>FillRectangleXY</v>
       </c>
-      <c r="G30" t="s">
+      <c r="I35" t="s">
         <v>49</v>
       </c>
-      <c r="H30" t="s">
+      <c r="J35" t="s">
         <v>76</v>
       </c>
-      <c r="I30" t="str">
+      <c r="K35" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;FillRectangleXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Fill a rectangle using two corners.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;FillRectangleXY&lt;/td&gt;&lt;td&gt;X1, Y1, X2, Y2&lt;/td&gt;&lt;td&gt;Fill a rectangle using two corners.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+        <v>MoveAngleLength</v>
+      </c>
+      <c r="I36" t="s">
+        <v>47</v>
+      </c>
+      <c r="J36" t="s">
+        <v>77</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;MoveAngleLength&lt;/td&gt;&lt;td&gt;X, Y, Angle, Length&lt;/td&gt;&lt;td&gt;Move the tool, without cutting, at an angle, by a specified length.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>40</v>
       </c>
-      <c r="B31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F31" t="str">
-        <f t="shared" si="0"/>
-        <v>MoveAngleLength</v>
-      </c>
-      <c r="G31" t="s">
-        <v>47</v>
-      </c>
-      <c r="H31" t="s">
-        <v>77</v>
-      </c>
-      <c r="I31" t="str">
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="H37" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;MoveAngleLength&lt;/td&gt;&lt;td&gt;X, Y, Angle, Length&lt;/td&gt;&lt;td&gt;Move the tool, without cutting, at an angle, by a specified length.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" t="s">
+        <v>MoveXY</v>
+      </c>
+      <c r="I37" t="s">
+        <v>50</v>
+      </c>
+      <c r="J37" t="s">
+        <v>78</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="2"/>
+        <v>&lt;tr&gt;&lt;td&gt;MoveXY&lt;/td&gt;&lt;td&gt;X, Y&lt;/td&gt;&lt;td&gt;Move the tool, without cutting, to the specified coordinate.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
         <v>32</v>
       </c>
-      <c r="F32" t="str">
-        <f t="shared" si="0"/>
-        <v>MoveXY</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="H38" t="str">
+        <f t="shared" si="1"/>
+        <v>PointXY</v>
+      </c>
+      <c r="I38" t="s">
         <v>50</v>
       </c>
-      <c r="H32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I32" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;MoveXY&lt;/td&gt;&lt;td&gt;X, Y&lt;/td&gt;&lt;td&gt;Move the tool, without cutting, to the specified coordinate.&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" t="str">
-        <f t="shared" si="0"/>
-        <v>PointXY</v>
-      </c>
-      <c r="G33" t="s">
-        <v>50</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="J38" t="s">
         <v>79</v>
       </c>
-      <c r="I33" t="str">
-        <f t="shared" si="1"/>
+      <c r="K38" t="str">
+        <f t="shared" si="2"/>
         <v>&lt;tr&gt;&lt;td&gt;PointXY&lt;/td&gt;&lt;td&gt;X, Y&lt;/td&gt;&lt;td&gt;Drill at a point represented by the X and Y coordinates.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I33" xr:uid="{4D95A485-D9E0-44E7-A352-6F438C309CFE}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="X, Y"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K38" xr:uid="{4D95A485-D9E0-44E7-A352-6F438C309CFE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C11D7ED-A239-4470-B308-11D637DC39C8}">
-  <dimension ref="A1:F23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C11D7ED-A239-4470-B308-11D637DC39C8}">
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -6797,472 +7214,641 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F31" si="0">CONCATENATE("public bool ShouldSerialize",B2,"()",CHAR(13),CHAR(10),"{",CHAR(13),CHAR(10),"return this.m",B2,"?.Length &gt; 0;",CHAR(13),CHAR(10),"}")</f>
+        <v>public bool ShouldSerializeOperationId()_x000D_
+{_x000D_
+return this.mOperationId?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeOperationName()_x000D_
+{_x000D_
+return this.mOperationName?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="F2" t="str">
-        <f>CONCATENATE("public bool ShouldSerialize",B2,"()",CHAR(13),CHAR(10),"{",CHAR(13),CHAR(10),"return true;",CHAR(13),CHAR(10),"}")</f>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
         <v>public bool ShouldSerializeAction()_x000D_
 {_x000D_
-return true;_x000D_
+return this.mAction?.Length &gt; 0;_x000D_
 }</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeStartOffsetX()_x000D_
+{_x000D_
+return this.mStartOffsetX?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeStartOffsetXOrigin()_x000D_
+{_x000D_
+return this.mStartOffsetXOrigin?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeStartOffsetY()_x000D_
+{_x000D_
+return this.mStartOffsetY?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeStartOffsetYOrigin()_x000D_
+{_x000D_
+return this.mStartOffsetYOrigin?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeDiameter()_x000D_
+{_x000D_
+return this.mDiameter?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeRadius()_x000D_
+{_x000D_
+return this.mRadius?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeDiameterX()_x000D_
+{_x000D_
+return this.mDiameterX?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeDiameterY()_x000D_
+{_x000D_
+return this.mDiameterY?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeRadiusX()_x000D_
+{_x000D_
+return this.mRadiusX?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeRadiusY()_x000D_
+{_x000D_
+return this.mRadiusY?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeOffsetX()_x000D_
+{_x000D_
+return this.mOffsetX?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeOffsetXOrigin()_x000D_
+{_x000D_
+return this.mOffsetXOrigin?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeOffsetY()_x000D_
+{_x000D_
+return this.mOffsetY?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeOffsetYOrigin()_x000D_
+{_x000D_
+return this.mOffsetYOrigin?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeEndOffsetX()_x000D_
+{_x000D_
+return this.mEndOffsetX?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeEndOffsetXOrigin()_x000D_
+{_x000D_
+return this.mEndOffsetXOrigin?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeEndOffsetY()_x000D_
+{_x000D_
+return this.mEndOffsetY?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeEndOffsetYOrigin()_x000D_
+{_x000D_
+return this.mEndOffsetYOrigin?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F23" si="0">CONCATENATE("public bool ShouldSerialize",B3,"()",CHAR(13),CHAR(10),"{",CHAR(13),CHAR(10),"return true;",CHAR(13),CHAR(10),"}")</f>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
         <v>public bool ShouldSerializeAngle()_x000D_
 {_x000D_
-return true;_x000D_
+return this.mAngle?.Length &gt; 0;_x000D_
 }</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeStartAngle()_x000D_
+{_x000D_
+return this.mStartAngle?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeEndAngle()_x000D_
+{_x000D_
+return this.mEndAngle?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeLength()_x000D_
+{_x000D_
+return this.mLength?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>public bool ShouldSerializeWidth()_x000D_
+{_x000D_
+return this.mWidth?.Length &gt; 0;_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F28" t="str">
         <f t="shared" si="0"/>
         <v>public bool ShouldSerializeDepth()_x000D_
 {_x000D_
-return true;_x000D_
+return this.mDepth?.Length &gt; 0;_x000D_
 }</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="F5" t="str">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeEndOffsetX()_x000D_
+        <v>public bool ShouldSerializeKerf()_x000D_
 {_x000D_
-return true;_x000D_
+return this.mKerf?.Length &gt; 0;_x000D_
 }</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="F6" t="str">
+    <row r="30" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeEndOffsetXOrigin()_x000D_
+        <v>public bool ShouldSerializeTool()_x000D_
 {_x000D_
-return true;_x000D_
+return this.mTool?.Length &gt; 0;_x000D_
 }</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeEndOffsetY()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeEndOffsetYOrigin()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>21</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="F9" t="str">
+      <c r="F31" t="str">
         <f t="shared" si="0"/>
         <v>public bool ShouldSerializeHiddenVariables()_x000D_
 {_x000D_
-return true;_x000D_
+return this.mHiddenVariables?.Length &gt; 0;_x000D_
 }</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeKerf()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeLength()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeOffsetX()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeOffsetXOrigin()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeOffsetY()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeOffsetYOrigin()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeOperationId()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeOperationName()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeStartOffsetX()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeStartOffsetXOrigin()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeStartOffsetY()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>6</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeStartOffsetYOrigin()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeTool()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>17</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeWidth()_x000D_
-{_x000D_
-return true;_x000D_
-}</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D24">
-    <sortCondition ref="B2:B24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F31">
+    <sortCondition ref="A2:A31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7525,11 +8111,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA889C0-613C-40F2-B26E-08804F9EC236}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -7562,307 +8148,433 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C2" t="s">
-        <v>398</v>
+        <v>420</v>
       </c>
       <c r="E2" t="s">
-        <v>440</v>
-      </c>
-      <c r="F2" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>421</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>420</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>423</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>415</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>396</v>
       </c>
       <c r="E4" t="s">
-        <v>416</v>
+        <v>424</v>
+      </c>
+      <c r="F4" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>417</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>396</v>
       </c>
       <c r="E5" t="s">
-        <v>441</v>
-      </c>
-      <c r="F5" t="s">
-        <v>438</v>
+        <v>591</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>418</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>396</v>
       </c>
       <c r="E6" t="s">
-        <v>410</v>
+        <v>593</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>419</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>396</v>
       </c>
       <c r="E7" t="s">
-        <v>442</v>
-      </c>
-      <c r="F7" t="s">
-        <v>439</v>
+        <v>594</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>408</v>
+        <v>607</v>
       </c>
       <c r="C8" t="s">
-        <v>396</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>435</v>
-      </c>
-      <c r="F8" t="s">
-        <v>436</v>
+        <v>611</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>396</v>
       </c>
       <c r="E9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C10" t="s">
-        <v>396</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>410</v>
+        <v>426</v>
       </c>
       <c r="F10" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="C11" t="s">
-        <v>175</v>
+        <v>396</v>
       </c>
       <c r="E11" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="C12" t="s">
-        <v>396</v>
+        <v>175</v>
       </c>
       <c r="E12" t="s">
-        <v>403</v>
+        <v>428</v>
+      </c>
+      <c r="F12" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>406</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
+      <c r="D13" t="s">
+        <v>386</v>
+      </c>
       <c r="E13" t="s">
-        <v>426</v>
-      </c>
-      <c r="F13" t="s">
-        <v>427</v>
+        <v>401</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>404</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
         <v>396</v>
       </c>
+      <c r="D14" t="str">
+        <f>"0"</f>
+        <v>0</v>
+      </c>
       <c r="E14" t="s">
-        <v>405</v>
+        <v>434</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C15" t="s">
-        <v>175</v>
+        <v>396</v>
       </c>
       <c r="E15" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="F15" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>411</v>
+      </c>
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
       <c r="E16" t="s">
-        <v>384</v>
+        <v>412</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>409</v>
       </c>
       <c r="C17" t="s">
         <v>396</v>
       </c>
-      <c r="D17" t="str">
-        <f>"0"</f>
-        <v>0</v>
-      </c>
       <c r="E17" t="s">
-        <v>434</v>
+        <v>410</v>
+      </c>
+      <c r="F17" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>413</v>
       </c>
       <c r="C18" t="s">
-        <v>396</v>
+        <v>175</v>
       </c>
       <c r="E18" t="s">
-        <v>424</v>
-      </c>
-      <c r="F18" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>422</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" t="s">
-        <v>386</v>
+        <v>398</v>
       </c>
       <c r="E19" t="s">
-        <v>401</v>
+        <v>440</v>
+      </c>
+      <c r="F19" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>396</v>
+      </c>
+      <c r="E20" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>396</v>
+      </c>
+      <c r="E21" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" t="s">
+        <v>396</v>
+      </c>
+      <c r="E22" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>606</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>415</v>
+      </c>
+      <c r="C24" t="s">
+        <v>396</v>
+      </c>
+      <c r="E24" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>417</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>441</v>
+      </c>
+      <c r="F25" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>418</v>
+      </c>
+      <c r="C26" t="s">
+        <v>396</v>
+      </c>
+      <c r="E26" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>419</v>
+      </c>
+      <c r="C27" t="s">
+        <v>175</v>
+      </c>
+      <c r="E27" t="s">
+        <v>442</v>
+      </c>
+      <c r="F27" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>397</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C28" t="s">
         <v>398</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D28" t="s">
         <v>399</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E28" t="s">
         <v>400</v>
       </c>
     </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>396</v>
+      </c>
+      <c r="E29" t="s">
+        <v>524</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
-    <sortCondition ref="A2:A20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
+    <sortCondition ref="B2:B29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates for version 25.1225.4218
</commit_message>
<xml_diff>
--- a/Docs/ShopToolsWorksheet.xlsx
+++ b/Docs/ShopToolsWorksheet.xlsx
@@ -8,32 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48df8f255f7bda56/Develop/Shared/ShopTools/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2327" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3AF5DD2-C24A-403D-9B37-CBDB4FC0EB36}"/>
+  <xr:revisionPtr revIDLastSave="2421" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC9FF105-415E-421C-AF41-02F2FDA47E8A}"/>
   <bookViews>
-    <workbookView xWindow="4452" yWindow="1908" windowWidth="17256" windowHeight="8964" firstSheet="14" activeTab="17" xr2:uid="{66387098-6DAB-4DD6-BA63-A47627A5E346}"/>
+    <workbookView xWindow="4452" yWindow="1908" windowWidth="17256" windowHeight="8964" firstSheet="15" activeTab="18" xr2:uid="{66387098-6DAB-4DD6-BA63-A47627A5E346}"/>
   </bookViews>
   <sheets>
     <sheet name="frmMain" sheetId="9" r:id="rId1"/>
     <sheet name="frmSettings" sheetId="8" r:id="rId2"/>
-    <sheet name="OperationActionPropertyItem" sheetId="16" r:id="rId3"/>
-    <sheet name="OperationActionTypes" sheetId="3" r:id="rId4"/>
-    <sheet name="PatternOperationItem" sheetId="17" r:id="rId5"/>
-    <sheet name="PatternTemplateItem" sheetId="6" r:id="rId6"/>
-    <sheet name="PatternTemplate.CutProfileItem" sheetId="19" r:id="rId7"/>
-    <sheet name="PatternTemplatePlotProperties" sheetId="12" r:id="rId8"/>
-    <sheet name="PlotPathItem" sheetId="5" r:id="rId9"/>
-    <sheet name="PropertyDefinitionItem" sheetId="13" r:id="rId10"/>
-    <sheet name="ShopToolsConfigItem" sheetId="7" r:id="rId11"/>
-    <sheet name="ToolPathItem" sheetId="1" r:id="rId12"/>
-    <sheet name="ToolPathSequenceStepItem" sheetId="2" r:id="rId13"/>
-    <sheet name="ToolTypeDefinitionItem" sheetId="11" r:id="rId14"/>
-    <sheet name="UserToolItem" sheetId="10" r:id="rId15"/>
-    <sheet name="Polarization" sheetId="15" r:id="rId16"/>
-    <sheet name="WorkpieceInfoItem" sheetId="18" r:id="rId17"/>
-    <sheet name="Work" sheetId="20" r:id="rId18"/>
+    <sheet name="OperationActionChecklist" sheetId="21" r:id="rId3"/>
+    <sheet name="OperationActionPropertyItem" sheetId="16" r:id="rId4"/>
+    <sheet name="OperationActionTypes" sheetId="3" r:id="rId5"/>
+    <sheet name="PatternOperationItem" sheetId="17" r:id="rId6"/>
+    <sheet name="PatternTemplateItem" sheetId="6" r:id="rId7"/>
+    <sheet name="PatternTemplate.CutProfileItem" sheetId="19" r:id="rId8"/>
+    <sheet name="PatternTemplatePlotProperties" sheetId="12" r:id="rId9"/>
+    <sheet name="PlotPathItem" sheetId="5" r:id="rId10"/>
+    <sheet name="PropertyDefinitionItem" sheetId="13" r:id="rId11"/>
+    <sheet name="ShopToolsConfigItem" sheetId="7" r:id="rId12"/>
+    <sheet name="ToolPathItem" sheetId="1" r:id="rId13"/>
+    <sheet name="ToolPathSequenceStepItem" sheetId="2" r:id="rId14"/>
+    <sheet name="ToolTypeDefinitionItem" sheetId="11" r:id="rId15"/>
+    <sheet name="UserToolItem" sheetId="10" r:id="rId16"/>
+    <sheet name="Polarization" sheetId="15" r:id="rId17"/>
+    <sheet name="WorkpieceInfoItem" sheetId="18" r:id="rId18"/>
+    <sheet name="Work" sheetId="20" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">OperationActionTypes!$A$1:$K$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">OperationActionTypes!$A$1:$K$38</definedName>
     <definedName name="polarizationLength">Polarization!$E$2</definedName>
     <definedName name="polarizationWidth">Polarization!$F$2</definedName>
     <definedName name="polarizationWkHeight">Polarization!$L$2</definedName>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="639">
   <si>
     <t>Name</t>
   </si>
@@ -1880,15 +1881,9 @@
     <t>End</t>
   </si>
   <si>
-    <t>X, Y, Radius, StartAngle, EndAngle</t>
-  </si>
-  <si>
     <t>Draw an arc using a center coordinate, an offset starting coordinate, and a sweep angle.</t>
   </si>
   <si>
-    <t>Draw an arc using a center coordinate, a radius, a start angle, and an end angle.</t>
-  </si>
-  <si>
     <t>X, Y, X1, Y1, Angle</t>
   </si>
   <si>
@@ -1901,21 +1896,12 @@
     <t>StartAngle</t>
   </si>
   <si>
-    <t>EndAngle</t>
-  </si>
-  <si>
     <t>The starting angle of the operation.</t>
   </si>
   <si>
-    <t>The ending angle of the operation.</t>
-  </si>
-  <si>
     <t>The angle at which the operation begins.</t>
   </si>
   <si>
-    <t>The angle at which the operation ends.</t>
-  </si>
-  <si>
     <t>Draw a rectangle using a center offset, length, and width.</t>
   </si>
   <si>
@@ -1947,6 +1933,69 @@
   </si>
   <si>
     <t>result</t>
+  </si>
+  <si>
+    <t>OperationActionEnum.cs</t>
+  </si>
+  <si>
+    <t>Operation action enumeration definition.</t>
+  </si>
+  <si>
+    <t>Conceptual definition.</t>
+  </si>
+  <si>
+    <t>ShopToolsWorksheet[OperationActionPropertyItem]</t>
+  </si>
+  <si>
+    <t>ShopToolsWorksheet[PatternOperationItem]</t>
+  </si>
+  <si>
+    <t>Prototype for associated properties.</t>
+  </si>
+  <si>
+    <t>ShopToolsWorksheet[OperationActionTypes]</t>
+  </si>
+  <si>
+    <t>ShopToolsWorksheet[PatternTemplatePlotProperties]</t>
+  </si>
+  <si>
+    <t>Configuration file prototype for associated properties.</t>
+  </si>
+  <si>
+    <t>Prototype for configuration class.</t>
+  </si>
+  <si>
+    <t>OperationActionProperty.cs</t>
+  </si>
+  <si>
+    <t>PatternOperation.cs</t>
+  </si>
+  <si>
+    <t>Sweep</t>
+  </si>
+  <si>
+    <t>X, Y, Radius, StartAngle, SweepAngle</t>
+  </si>
+  <si>
+    <t>Draw an arc using a center coordinate, a radius, a start angle, and a sweep angle.</t>
+  </si>
+  <si>
+    <t>SweepAngle</t>
+  </si>
+  <si>
+    <t>The angle to sweep on the operation.</t>
+  </si>
+  <si>
+    <t>The sweep angle for the operation.</t>
+  </si>
+  <si>
+    <t>OperationLayout.cs</t>
+  </si>
+  <si>
+    <t>Sweep Forward</t>
+  </si>
+  <si>
+    <t>Sweep Reverse</t>
   </si>
 </sst>
 </file>
@@ -1982,7 +2031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1990,7 +2039,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3318,6 +3366,155 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F827F6A-76EE-4E0B-A235-424AC93E8143}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D11">
+    <sortCondition ref="B2:B11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9058CEE2-BBBB-4F29-AFA7-F294F0A7F9F2}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3412,7 +3609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953F205B-2C58-4122-A2D3-8F3ECB83AFB9}">
   <dimension ref="A1:E21"/>
   <sheetViews>
@@ -3777,7 +3974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D4860C-5313-40BA-BA7E-963DF1D1F2FA}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -3914,7 +4111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0294DF1A-89F9-416C-809D-FBC7C35CED92}">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -4218,7 +4415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3067B038-5D30-4C7C-B6D5-51DDD972B634}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -4310,7 +4507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF6DC55-361C-4068-830E-78999229E0B8}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -4404,7 +4601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A9CED-8EE1-4F59-96AD-E0D93BEB7D28}">
   <dimension ref="B1:Q5"/>
   <sheetViews>
@@ -4578,7 +4775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE611F5F-3661-476E-B802-055B6AF9BB39}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -4911,13 +5108,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E40DB11-6C4A-49D6-826F-B66B6B7A1415}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -5124,7 +5321,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="B7">
         <v>1454</v>
@@ -5135,7 +5332,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="B8">
         <v>1454</v>
@@ -5146,7 +5343,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="B9">
         <v>1302</v>
@@ -5157,7 +5354,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="B11">
         <f>B8-B7</f>
@@ -5170,7 +5367,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="B12">
         <f>B9-B7</f>
@@ -5183,7 +5380,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="B14">
         <f>B11*B11+C11*C11</f>
@@ -5192,25 +5389,25 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="B15">
         <f>B12*B11+C12*C11</f>
         <v>103378</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="B17">
         <f>B15/B14</f>
         <v>1.6023622047244095</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="B19">
         <f>B7+B11*B17</f>
@@ -5221,7 +5418,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1454.23</v>
       </c>
@@ -5236,7 +5433,7 @@
         <v>1454.23</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>203</v>
       </c>
@@ -5249,6 +5446,108 @@
       <c r="E23">
         <f>A23+B23*C23</f>
         <v>609.40000000000009</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>598</v>
+      </c>
+      <c r="B26">
+        <v>47</v>
+      </c>
+      <c r="C26">
+        <f>B26</f>
+        <v>47</v>
+      </c>
+      <c r="F26">
+        <v>320</v>
+      </c>
+      <c r="G26">
+        <f>F26</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>599</v>
+      </c>
+      <c r="B27">
+        <v>320</v>
+      </c>
+      <c r="C27">
+        <f>IF(B26&gt;B27,B27+360,B27)</f>
+        <v>320</v>
+      </c>
+      <c r="D27">
+        <f>C27-C26</f>
+        <v>273</v>
+      </c>
+      <c r="F27">
+        <v>47</v>
+      </c>
+      <c r="G27">
+        <f>IF(F26&gt;F27,F27+360,F27)</f>
+        <v>407</v>
+      </c>
+      <c r="H27">
+        <f>G27-G26</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>598</v>
+      </c>
+      <c r="B30">
+        <v>47</v>
+      </c>
+      <c r="C30">
+        <f>IF(B31&gt;B30,B30+360,B30)</f>
+        <v>407</v>
+      </c>
+      <c r="F30">
+        <v>320</v>
+      </c>
+      <c r="G30">
+        <f>IF(F31&gt;F30,F30+360,F30)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>599</v>
+      </c>
+      <c r="B31">
+        <v>320</v>
+      </c>
+      <c r="C31">
+        <f>B31</f>
+        <v>320</v>
+      </c>
+      <c r="D31">
+        <f>C31-C30</f>
+        <v>-87</v>
+      </c>
+      <c r="F31">
+        <v>47</v>
+      </c>
+      <c r="G31">
+        <f>F31</f>
+        <v>47</v>
+      </c>
+      <c r="H31">
+        <f>G31-G30</f>
+        <v>-273</v>
       </c>
     </row>
   </sheetData>
@@ -5999,6 +6298,88 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E96C129-99DA-4677-BD83-78A82FA1CBD9}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>618</v>
+      </c>
+      <c r="B2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>621</v>
+      </c>
+      <c r="B3" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>624</v>
+      </c>
+      <c r="B4" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>622</v>
+      </c>
+      <c r="B5" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>625</v>
+      </c>
+      <c r="B6" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>636</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B3BBD0-6A83-4733-8619-CAD7D79AE6BF}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -6117,13 +6498,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D95A485-D9E0-44E7-A352-6F438C309CFE}">
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -6132,7 +6513,7 @@
     <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.21875" customWidth="1"/>
     <col min="8" max="8" width="28.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.6640625" bestFit="1" customWidth="1"/>
@@ -6177,10 +6558,10 @@
         <v>DrawArcCenterOffsetXY</v>
       </c>
       <c r="I2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="J2" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="K2" t="str">
         <f>CONCATENATE("&lt;tr&gt;&lt;td&gt;",H2,"&lt;/td&gt;&lt;td&gt;",I2,"&lt;/td&gt;&lt;td&gt;",J2,"&lt;/td&gt;&lt;/tr&gt;")</f>
@@ -6211,10 +6592,10 @@
         <v>DrawArcCenterOffsetXYAngle</v>
       </c>
       <c r="I3" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="J3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K4" si="0">CONCATENATE("&lt;tr&gt;&lt;td&gt;",H3,"&lt;/td&gt;&lt;td&gt;",I3,"&lt;/td&gt;&lt;td&gt;",J3,"&lt;/td&gt;&lt;/tr&gt;")</f>
@@ -6238,24 +6619,24 @@
         <v>598</v>
       </c>
       <c r="F4" t="s">
-        <v>599</v>
+        <v>630</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
       </c>
       <c r="H4" t="str">
         <f>CONCATENATE(A4,B4,C4,D4,E4,F4,G4)</f>
-        <v>DrawArcCenterRadiusStartEndAngle</v>
+        <v>DrawArcCenterRadiusStartSweepAngle</v>
       </c>
       <c r="I4" t="s">
-        <v>600</v>
+        <v>631</v>
       </c>
       <c r="J4" t="s">
-        <v>602</v>
+        <v>632</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;DrawArcCenterRadiusStartEndAngle&lt;/td&gt;&lt;td&gt;X, Y, Radius, StartAngle, EndAngle&lt;/td&gt;&lt;td&gt;Draw an arc using a center coordinate, a radius, a start angle, and an end angle.&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;DrawArcCenterRadiusStartSweepAngle&lt;/td&gt;&lt;td&gt;X, Y, Radius, StartAngle, SweepAngle&lt;/td&gt;&lt;td&gt;Draw an arc using a center coordinate, a radius, a start angle, and a sweep angle.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -6639,32 +7020,30 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3" t="str">
+      <c r="H19" t="str">
         <f t="shared" si="1"/>
         <v>DrawRectangleCenterLengthWidth</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" t="s">
         <v>48</v>
       </c>
       <c r="J19" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="2"/>
@@ -7024,32 +7403,30 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="A33" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3" t="str">
+      <c r="H33" t="str">
         <f t="shared" si="1"/>
         <v>FillRectangleCenterLengthWidth</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I33" t="s">
         <v>48</v>
       </c>
       <c r="J33" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -7181,13 +7558,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C11D7ED-A239-4470-B308-11D637DC39C8}">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -7679,13 +8056,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>513</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
@@ -7700,19 +8077,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>607</v>
+        <v>633</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>513</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>609</v>
+        <v>635</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>public bool ShouldSerializeEndAngle()_x000D_
+        <v>public bool ShouldSerializeSweepAngle()_x000D_
 {_x000D_
-return this.mEndAngle?.Length &gt; 0;_x000D_
+return this.mSweepAngle?.Length &gt; 0;_x000D_
 }</v>
       </c>
     </row>
@@ -7852,12 +8229,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5D5A8F-5DB5-46AB-891B-99181D46233D}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -8045,7 +8422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B73DC4-995B-4AB7-99BA-A9CF8C63FFB2}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -8109,13 +8486,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA889C0-613C-40F2-B26E-08804F9EC236}">
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -8238,13 +8615,13 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>607</v>
+        <v>633</v>
       </c>
       <c r="C8" t="s">
         <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>611</v>
+        <v>634</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -8470,13 +8847,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C23" t="s">
         <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -8578,153 +8955,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F827F6A-76EE-4E0B-A235-424AC93E8143}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D11">
-    <sortCondition ref="B2:B11"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates for version 25.2310.3903
README updated; Form-level SDK documentation added from previous version; About box added.
</commit_message>
<xml_diff>
--- a/Docs/ShopToolsWorksheet.xlsx
+++ b/Docs/ShopToolsWorksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48df8f255f7bda56/Develop/Shared/ShopTools/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2760" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{991857D0-46E3-49FA-8C9C-F887C35482C1}"/>
+  <xr:revisionPtr revIDLastSave="2774" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60297B9F-A7A9-45E4-9B50-A1F53A11F876}"/>
   <bookViews>
-    <workbookView xWindow="4452" yWindow="1908" windowWidth="17256" windowHeight="8964" xr2:uid="{66387098-6DAB-4DD6-BA63-A47627A5E346}"/>
+    <workbookView xWindow="4452" yWindow="1908" windowWidth="17256" windowHeight="8964" firstSheet="16" activeTab="19" xr2:uid="{66387098-6DAB-4DD6-BA63-A47627A5E346}"/>
   </bookViews>
   <sheets>
     <sheet name="frmEditTemplates" sheetId="22" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="719">
   <si>
     <t>Name</t>
   </si>
@@ -2228,6 +2228,15 @@
   </si>
   <si>
     <t>btnOperationDelete</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>CX</t>
+  </si>
+  <si>
+    <t>CY</t>
   </si>
 </sst>
 </file>
@@ -2621,7 +2630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1870BC-8EC7-44DD-82C7-809BB8605A7E}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
@@ -6724,11 +6733,11 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E40DB11-6C4A-49D6-826F-B66B6B7A1415}">
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -7274,6 +7283,58 @@
       </c>
       <c r="B47">
         <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" t="s">
+        <v>669</v>
+      </c>
+      <c r="D49" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>922.85699999999997</v>
+      </c>
+      <c r="B50">
+        <v>117.143</v>
+      </c>
+      <c r="C50">
+        <v>468.57100000000003</v>
+      </c>
+      <c r="D50">
+        <v>222.857</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>717</v>
+      </c>
+      <c r="B52">
+        <f>A50+(C50/2)</f>
+        <v>1157.1424999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>718</v>
+      </c>
+      <c r="B53">
+        <f>B50+(D50/2)</f>
+        <v>228.57150000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f>360/36</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to ShopTools reference configuration
In preparation for material type-driven feed rate settings.
</commit_message>
<xml_diff>
--- a/Docs/ShopToolsWorksheet.xlsx
+++ b/Docs/ShopToolsWorksheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48df8f255f7bda56/Develop/Shared/ShopTools/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2774" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60297B9F-A7A9-45E4-9B50-A1F53A11F876}"/>
+  <xr:revisionPtr revIDLastSave="2826" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31A0522E-E2DA-4931-8489-57D5EA07E16D}"/>
   <bookViews>
     <workbookView xWindow="4452" yWindow="1908" windowWidth="17256" windowHeight="8964" firstSheet="16" activeTab="19" xr2:uid="{66387098-6DAB-4DD6-BA63-A47627A5E346}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="732">
   <si>
     <t>Name</t>
   </si>
@@ -2237,6 +2237,45 @@
   </si>
   <si>
     <t>CY</t>
+  </si>
+  <si>
+    <t>Left:</t>
+  </si>
+  <si>
+    <t>Button 1</t>
+  </si>
+  <si>
+    <t>Button 2</t>
+  </si>
+  <si>
+    <t>Button 3</t>
+  </si>
+  <si>
+    <t>Center:</t>
+  </si>
+  <si>
+    <t>MaterialTypeName</t>
+  </si>
+  <si>
+    <t>The material selected for this cut.</t>
+  </si>
+  <si>
+    <t>MaterialTypes</t>
+  </si>
+  <si>
+    <t>MaterialTypeCollection</t>
+  </si>
+  <si>
+    <t>Collection of material types defined in this session.</t>
+  </si>
+  <si>
+    <t>Top:</t>
+  </si>
+  <si>
+    <t>Top Next:</t>
+  </si>
+  <si>
+    <t>Distance:</t>
   </si>
 </sst>
 </file>
@@ -4254,11 +4293,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953F205B-2C58-4122-A2D3-8F3ECB83AFB9}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -4320,38 +4359,38 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>142</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>142</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
@@ -4371,46 +4410,47 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>0</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>155</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
@@ -4418,30 +4458,27 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -4449,16 +4486,16 @@
         <v>140</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>165</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -4466,16 +4503,16 @@
         <v>140</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>165</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -4483,136 +4520,156 @@
         <v>140</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>198</v>
-      </c>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>176</v>
+        <v>7</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>7</v>
+        <v>176</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>202</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E23">
+    <sortCondition ref="B2:B23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5420,11 +5477,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE611F5F-3661-476E-B802-055B6AF9BB39}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -5563,7 +5620,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>532</v>
@@ -5576,17 +5633,17 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>140</v>
+      <c r="A11" s="1">
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>535</v>
+        <v>724</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>536</v>
+        <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>537</v>
+        <v>725</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -5594,94 +5651,94 @@
         <v>140</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>540</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>549</v>
+        <v>169</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>504</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>504</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>547</v>
@@ -5689,57 +5746,71 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>504</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>504</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>558</v>
       </c>
     </row>
@@ -6733,11 +6804,11 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E40DB11-6C4A-49D6-826F-B66B6B7A1415}">
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -7335,6 +7406,96 @@
       <c r="A56">
         <f>360/36</f>
         <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>719</v>
+      </c>
+      <c r="B59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>317</v>
+      </c>
+      <c r="B60">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>719</v>
+      </c>
+      <c r="B62">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>317</v>
+      </c>
+      <c r="B64">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>723</v>
+      </c>
+      <c r="B65">
+        <f>B62-((B62-(B59+B60))/2)</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>719</v>
+      </c>
+      <c r="B66">
+        <f>B65-(B64/2)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>729</v>
+      </c>
+      <c r="B69">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>730</v>
+      </c>
+      <c r="B70">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>731</v>
+      </c>
+      <c r="B71">
+        <f>B70-B69</f>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for version 25.2409.5030
## Bugs Fixed
 - Bug: Cut edit form storing starting position 2X below its defined location.
 - Bug: Cut edit form not displaying first start coordinate.
 - Bug: Manually defined transits should always count in output.
 - Test: Check all configurations in ShopToolsUtil.TransformToAbsolute.

## Improvements Completed
 - Provide 3D preview of the rendered path.
 - Set a default thickness for materials.
</commit_message>
<xml_diff>
--- a/Docs/ShopToolsWorksheet.xlsx
+++ b/Docs/ShopToolsWorksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48df8f255f7bda56/Develop/Shared/ShopTools/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2826" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31A0522E-E2DA-4931-8489-57D5EA07E16D}"/>
+  <xr:revisionPtr revIDLastSave="3011" documentId="8_{4907CCD6-D35A-4B08-9D58-0AC4D98F8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13B57DCD-DA03-4F02-A401-68D366AD0387}"/>
   <bookViews>
     <workbookView xWindow="4452" yWindow="1908" windowWidth="17256" windowHeight="8964" firstSheet="16" activeTab="19" xr2:uid="{66387098-6DAB-4DD6-BA63-A47627A5E346}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="759">
   <si>
     <t>Name</t>
   </si>
@@ -2276,6 +2276,87 @@
   </si>
   <si>
     <t>Distance:</t>
+  </si>
+  <si>
+    <t>Bottom:</t>
+  </si>
+  <si>
+    <t>Dimension:</t>
+  </si>
+  <si>
+    <t>Bottom/Up</t>
+  </si>
+  <si>
+    <t>Center/Dn</t>
+  </si>
+  <si>
+    <t>Center/Up</t>
+  </si>
+  <si>
+    <t>Bottom/Dn</t>
+  </si>
+  <si>
+    <t>Top/Dn</t>
+  </si>
+  <si>
+    <t>Top/Up</t>
+  </si>
+  <si>
+    <t>Drw Top:</t>
+  </si>
+  <si>
+    <t>Drw Bot:</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Convert Range</t>
+  </si>
+  <si>
+    <t>fromMin</t>
+  </si>
+  <si>
+    <t>toMin</t>
+  </si>
+  <si>
+    <t>fromMax</t>
+  </si>
+  <si>
+    <t>toMax</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>fromRange</t>
+  </si>
+  <si>
+    <t>toRange</t>
+  </si>
+  <si>
+    <t>Layer</t>
+  </si>
+  <si>
+    <t>Segments</t>
+  </si>
+  <si>
+    <t>PointB</t>
+  </si>
+  <si>
+    <t>{0.000,0.000,24.994}</t>
+  </si>
+  <si>
+    <t>{0.000,317.500,24.994}</t>
+  </si>
+  <si>
+    <t>{0.000,317.500,3.175}</t>
+  </si>
+  <si>
+    <t>{0.000,317.500,1.588}</t>
+  </si>
+  <si>
+    <t>Plunge</t>
   </si>
 </sst>
 </file>
@@ -6804,11 +6885,11 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E40DB11-6C4A-49D6-826F-B66B6B7A1415}">
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:Q106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -7455,7 +7536,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>723</v>
       </c>
@@ -7464,7 +7545,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>719</v>
       </c>
@@ -7473,7 +7554,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>729</v>
       </c>
@@ -7481,7 +7562,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>730</v>
       </c>
@@ -7489,13 +7570,409 @@
         <v>166</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>731</v>
       </c>
       <c r="B71">
         <f>B70-B69</f>
         <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>733</v>
+      </c>
+      <c r="B74">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>737</v>
+      </c>
+      <c r="C76" t="s">
+        <v>734</v>
+      </c>
+      <c r="D76" t="s">
+        <v>735</v>
+      </c>
+      <c r="E76" t="s">
+        <v>736</v>
+      </c>
+      <c r="F76" t="s">
+        <v>738</v>
+      </c>
+      <c r="G76" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>729</v>
+      </c>
+      <c r="B77">
+        <f>0-B74</f>
+        <v>-100</v>
+      </c>
+      <c r="C77">
+        <f>B74</f>
+        <v>100</v>
+      </c>
+      <c r="D77">
+        <f>0-(B74/2)</f>
+        <v>-50</v>
+      </c>
+      <c r="E77">
+        <f>B74/2</f>
+        <v>50</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>732</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <f>B74/2</f>
+        <v>50</v>
+      </c>
+      <c r="E78">
+        <f>0-(B74/2)</f>
+        <v>-50</v>
+      </c>
+      <c r="F78">
+        <f>B74</f>
+        <v>100</v>
+      </c>
+      <c r="G78">
+        <f>0-B74</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>740</v>
+      </c>
+      <c r="B80">
+        <f>B74</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>741</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>742</v>
+      </c>
+      <c r="B84">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>744</v>
+      </c>
+      <c r="B85">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>746</v>
+      </c>
+      <c r="B86">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>745</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>747</v>
+      </c>
+      <c r="B88">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>749</v>
+      </c>
+      <c r="B89">
+        <f>B86-B85</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>750</v>
+      </c>
+      <c r="B90">
+        <f>B88-B87</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>748</v>
+      </c>
+      <c r="B91">
+        <f>(((B84-B85)*B90)/B89)+B87</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>751</v>
+      </c>
+      <c r="C94" t="s">
+        <v>588</v>
+      </c>
+      <c r="F94" t="s">
+        <v>589</v>
+      </c>
+      <c r="I94" t="s">
+        <v>147</v>
+      </c>
+      <c r="K94" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>317.5</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="K95" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>317.5</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="I96">
+        <v>1.5874999999999999</v>
+      </c>
+      <c r="K96" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="F97">
+        <v>165.1</v>
+      </c>
+      <c r="G97">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="I97">
+        <v>1.5874999999999999</v>
+      </c>
+      <c r="K97" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>165.1</v>
+      </c>
+      <c r="D98">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="F98">
+        <v>165.1</v>
+      </c>
+      <c r="G98">
+        <v>-317.5</v>
+      </c>
+      <c r="I98">
+        <v>1.5874999999999999</v>
+      </c>
+      <c r="K98" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>165.1</v>
+      </c>
+      <c r="D99">
+        <v>-317.5</v>
+      </c>
+      <c r="F99">
+        <v>165.1</v>
+      </c>
+      <c r="G99">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="I99">
+        <v>3.1749999999999998</v>
+      </c>
+      <c r="K99" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>165.1</v>
+      </c>
+      <c r="D100">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="I100">
+        <v>3.1749999999999998</v>
+      </c>
+      <c r="K100" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>1</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>317.5</v>
+      </c>
+      <c r="I101">
+        <v>3.1749999999999998</v>
+      </c>
+      <c r="K101" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>752</v>
+      </c>
+      <c r="B103" t="s">
+        <v>599</v>
+      </c>
+      <c r="E103" t="s">
+        <v>753</v>
+      </c>
+      <c r="H103" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>754</v>
+      </c>
+      <c r="E104" t="s">
+        <v>755</v>
+      </c>
+      <c r="H104" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>755</v>
+      </c>
+      <c r="E105" t="s">
+        <v>756</v>
+      </c>
+      <c r="H105" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>756</v>
+      </c>
+      <c r="E106" t="s">
+        <v>757</v>
+      </c>
+      <c r="H106" t="s">
+        <v>758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>